<commit_message>
Update LinkML generated files
</commit_message>
<xml_diff>
--- a/project/excel/ak_schema.xlsx
+++ b/project/excel/ak_schema.xlsx
@@ -1,15 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Investigation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="InvestigationCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Container" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Investigation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reference" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Arm" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Participant" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StudyEvent" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LifeEvent" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImmuneExposure" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assessment" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specimen" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dataset" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Conclusion" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,17 +436,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>investigations</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>references</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>arms</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>study_events</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>participants</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>life_events</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>immune_exposures</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>assessments</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>specimens</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>assays</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>conclusions</t>
         </is>
       </c>
     </row>
@@ -445,7 +500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -462,22 +517,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>life_event</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>specimen_type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>tissue</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>process</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -497,22 +552,17 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,7 +573,652 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>specimen</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assay_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>target_entity_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assessments</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assays</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>investigations</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>data_location_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>data_location_value</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>organism</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>experiment_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Homo sapiens (human),Mus musculus (mouse)"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>investigations</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>issue</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>journal</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>pages</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>investigation</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>arm</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>biological_sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ethnicity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>geolocation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Homo sapiens (human),Mus musculus (mouse)"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"female,male"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"American Indian or Alaska Native,Asian,Black or African American,Native Hawaiian or Other Pacific Islander,White,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Hispanic or Latino,Not Hispanic or Latino,Other"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>arms</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>participant</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>study_event</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>life_event_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>geolocation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>t0_event</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>t0_event_type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>time_unit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Documented exposure without evidence for disease,Environmental exposure to endemic/ubiquitous agent without evidence for disease,Exposure with existing immune reactivity without evidence for disease,specimen collection"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>life_event</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>exposure_material</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>disease</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>disease_stage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>disease_severity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Influenza A virus,Mycobacterium tuberculosis,Plasmodium falciparum,Human gammaherpesvirus 4,Human betaherpesvirus 5,Diphtheria-Tetanus-Pertussis vaccine,Dryvax"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"healthy,COVID-19,Plasmodium falciparum malaria,dengue hemorrhagic fever"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"acute disease course,post disease course,unknown disease course,chronic disease course,other disease course"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>life_event</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assessment_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>target_entity_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>